<commit_message>
Remove results for vowpal; add for lightwood
</commit_message>
<xml_diff>
--- a/results/binary.xlsx
+++ b/results/binary.xlsx
@@ -467,27 +467,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.836 (0.832 Â± 0.002)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.964 (0.964 Â± 0.000)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.000)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.670 (0.616 Â± 0.039)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.983 (0.981 Â± 0.002)</t>
         </is>
       </c>
     </row>
@@ -499,27 +499,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.804 (0.744 Â± 0.029)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.966 (0.956 Â± 0.005)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.995 Â± 0.005)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.926 (0.685 Â± 0.162)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.966 Â± 0.017)</t>
         </is>
       </c>
     </row>
@@ -531,27 +531,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.829 (0.729 Â± 0.044)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.944 (0.918 Â± 0.010)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.000)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.719 (0.571 Â± 0.116)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.971 Â± 0.013)</t>
         </is>
       </c>
     </row>
@@ -563,27 +563,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.794 (0.747 Â± 0.035)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.964 (0.953 Â± 0.007)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.999 Â± 0.003)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.597 (0.519 Â± 0.056)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.991 (0.961 Â± 0.020)</t>
         </is>
       </c>
     </row>
@@ -595,27 +595,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.800 (0.760 Â± 0.024)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.975 (0.958 Â± 0.006)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.001)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.000)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.976 Â± 0.014)</t>
         </is>
       </c>
     </row>
@@ -627,27 +627,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.815 (0.738 Â± 0.039)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.959 (0.948 Â± 0.007)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.956 (0.932 Â± 0.013)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.946 (0.918 Â± 0.015)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.970 Â± 0.014)</t>
         </is>
       </c>
     </row>
@@ -691,27 +691,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.782 (0.745 Â± 0.032)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.971 (0.958 Â± 0.005)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.997 Â± 0.004)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.880 (0.834 Â± 0.037)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.991 (0.964 Â± 0.021)</t>
         </is>
       </c>
     </row>
@@ -723,27 +723,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.793 (0.748 Â± 0.032)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.970 (0.954 Â± 0.007)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.999 Â± 0.002)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (0.988 Â± 0.012)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.991 (0.971 Â± 0.015)</t>
         </is>
       </c>
     </row>
@@ -755,27 +755,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.794 (0.712 Â± 0.064)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.939 (0.888 Â± 0.028)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.890 (0.701 Â± 0.154)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.380 (0.347 Â± 0.022)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.966 (0.934 Â± 0.024)</t>
         </is>
       </c>
     </row>
@@ -787,27 +787,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.231 (0.176 Â± 0.024)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.244 (0.227 Â± 0.013)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.463 (0.399 Â± 0.030)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.368 (0.334 Â± 0.023)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.267 (0.192 Â± 0.037)</t>
         </is>
       </c>
     </row>
@@ -915,27 +915,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.801 (0.758 Â± 0.021)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.969 (0.957 Â± 0.005)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.001)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.971 (0.960 Â± 0.010)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.991 (0.970 Â± 0.016)</t>
         </is>
       </c>
     </row>
@@ -947,27 +947,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.792 (0.748 Â± 0.029)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.971 (0.954 Â± 0.006)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1.000 (1.000 Â± 0.000)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.992 (0.973 Â± 0.015)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>0.991 (0.963 Â± 0.020)</t>
         </is>
       </c>
     </row>
@@ -1020,27 +1020,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:54 (00:01:37 Â± 00:00:46)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:02 (00:04:33 Â± 00:00:12)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:44 (00:02:51 Â± 00:01:34)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:31 (00:04:59 Â± 00:00:23)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:01:41 (00:03:51 Â± 00:00:57)</t>
         </is>
       </c>
     </row>
@@ -1052,27 +1052,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:10 (00:00:22 Â± 00:00:09)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:38 (00:01:20 Â± 00:00:21)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:07 (00:00:11 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:11 (00:00:17 Â± 00:00:04)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:05 (00:00:06 Â± 00:00:02)</t>
         </is>
       </c>
     </row>
@@ -1084,27 +1084,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:16 (00:00:23 Â± 00:00:08)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:01:40 (00:02:04 Â± 00:00:23)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:30 (00:00:38 Â± 00:00:06)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:27 (00:00:43 Â± 00:00:08)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:18 (00:00:28 Â± 00:00:10)</t>
         </is>
       </c>
     </row>
@@ -1116,27 +1116,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:07 (00:05:14 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:07 (00:05:14 Â± 00:00:04)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:06 (00:05:12 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:07 (00:05:13 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:06 (00:05:12 Â± 00:00:03)</t>
         </is>
       </c>
     </row>
@@ -1148,27 +1148,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:55 (00:05:00 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:57 (00:05:01 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:57 (00:05:01 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:57 (00:04:59 Â± 00:00:01)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:56 (00:05:00 Â± 00:00:02)</t>
         </is>
       </c>
     </row>
@@ -1180,27 +1180,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:05 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:00 (00:05:04 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:00 (00:05:04 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:04 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:00 (00:05:01 Â± 00:00:01)</t>
         </is>
       </c>
     </row>
@@ -1244,27 +1244,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:00 (00:05:02 Â± 00:00:02)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:59 (00:05:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1276,27 +1276,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:18 (00:04:16 Â± 00:00:54)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:29 (00:04:29 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:29 (00:04:29 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:29 (00:04:33 Â± 00:00:05)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:04:29 (00:04:29 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1308,27 +1308,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:02 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:06 (00:05:06 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:05 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:02 (00:05:03 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:04 Â± 00:00:01)</t>
         </is>
       </c>
     </row>
@@ -1340,27 +1340,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:03:02 (00:03:12 Â± 00:00:06)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:02:13 (00:02:38 Â± 00:00:10)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:02:53 (00:03:13 Â± 00:00:07)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:02:29 (00:03:09 Â± 00:00:18)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:02:44 (00:03:05 Â± 00:00:07)</t>
         </is>
       </c>
     </row>
@@ -1468,27 +1468,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:11:09 (00:11:41 Â± 00:00:19)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:19:38 (00:20:31 Â± 00:00:34)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:13:36 (00:14:09 Â± 00:00:19)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:24 (00:11:41 Â± 00:06:14)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:09:40 (00:10:20 Â± 00:00:20)</t>
         </is>
       </c>
     </row>
@@ -1500,27 +1500,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:00 (00:05:06 Â± 00:00:08)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:02 (00:05:26 Â± 00:00:16)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:18 Â± 00:00:13)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:06 (00:05:28 Â± 00:00:13)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:05:01 (00:05:07 Â± 00:00:05)</t>
         </is>
       </c>
     </row>
@@ -1573,27 +1573,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:07 (00:00:08 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:08 (00:00:13 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:05 (00:00:06 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:05 (00:00:13 Â± 00:00:05)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:03 (00:00:13 Â± 00:00:03)</t>
         </is>
       </c>
     </row>
@@ -1605,27 +1605,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1637,27 +1637,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:01 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1669,27 +1669,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:02 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:02 Â± 00:00:01)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:02 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:02 Â± 00:00:01)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:01 (00:00:02 Â± 00:00:01)</t>
         </is>
       </c>
     </row>
@@ -1701,27 +1701,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:02 (00:00:06 Â± 00:00:03)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:01 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:01 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1733,27 +1733,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1797,27 +1797,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1829,27 +1829,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1861,27 +1861,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -1893,27 +1893,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -2021,27 +2021,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -2053,27 +2053,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>00:00:00 (00:00:00 Â± 00:00:00)</t>
         </is>
       </c>
     </row>
@@ -2126,27 +2126,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2158,27 +2158,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2190,27 +2190,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2222,27 +2222,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2254,27 +2254,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2286,27 +2286,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2350,27 +2350,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2382,27 +2382,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2414,27 +2414,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2446,27 +2446,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2574,27 +2574,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2606,27 +2606,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2677,30 +2677,20 @@
           <t>4intelligence</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -2709,30 +2699,20 @@
           <t>autogluon</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B3" t="n">
+        <v>23</v>
+      </c>
+      <c r="C3" t="n">
+        <v>41</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3" t="n">
+        <v>47</v>
+      </c>
+      <c r="F3" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -2741,30 +2721,20 @@
           <t>autokeras</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B4" t="n">
+        <v>23</v>
+      </c>
+      <c r="C4" t="n">
+        <v>31</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>41</v>
+      </c>
+      <c r="F4" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="5">
@@ -2773,30 +2743,20 @@
           <t>autopytorch</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B5" t="n">
+        <v>43</v>
+      </c>
+      <c r="C5" t="n">
+        <v>41</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>41</v>
+      </c>
+      <c r="F5" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="6">
@@ -2805,30 +2765,20 @@
           <t>autosklearn</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>41</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -2837,30 +2787,20 @@
           <t>evalml</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B7" t="n">
+        <v>23</v>
+      </c>
+      <c r="C7" t="n">
+        <v>41</v>
+      </c>
+      <c r="D7" t="n">
+        <v>37</v>
+      </c>
+      <c r="E7" t="n">
+        <v>23</v>
+      </c>
+      <c r="F7" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
@@ -2891,30 +2831,20 @@
           <t>flaml</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>31</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>31</v>
+      </c>
+      <c r="F9" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="10">
@@ -2923,30 +2853,20 @@
           <t>gama</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B10" t="n">
+        <v>41</v>
+      </c>
+      <c r="C10" t="n">
+        <v>41</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="11">
@@ -2955,30 +2875,20 @@
           <t>h2o</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+      <c r="D11" t="n">
+        <v>61</v>
+      </c>
+      <c r="E11" t="n">
+        <v>47</v>
+      </c>
+      <c r="F11" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="12">
@@ -2987,30 +2897,20 @@
           <t>lightautoml</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>41</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13</v>
+      </c>
+      <c r="F12" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -3085,30 +2985,20 @@
           <t>pycaret</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B16" t="n">
+        <v>23</v>
+      </c>
+      <c r="C16" t="n">
+        <v>41</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>47</v>
+      </c>
+      <c r="F16" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="17">
@@ -3117,30 +3007,20 @@
           <t>tpot</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="B17" t="n">
+        <v>23</v>
+      </c>
+      <c r="C17" t="n">
+        <v>41</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>61</v>
+      </c>
+      <c r="F17" t="n">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>